<commit_message>
read first sheet of excel
</commit_message>
<xml_diff>
--- a/data/price_list.xlsx
+++ b/data/price_list.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="価格リスト" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>